<commit_message>
Updated Unity file with map and Draft Presentation
</commit_message>
<xml_diff>
--- a/Sprint/Jira.xlsx
+++ b/Sprint/Jira.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheEnterpriseV2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheEnterpriseV2/Desktop/Actual Git/Sprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A3:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,10 +901,10 @@
       <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="J29" t="s">
@@ -912,28 +912,28 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
+      <c r="G32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>